<commit_message>
feat: delete upload file
</commit_message>
<xml_diff>
--- a/tests/Import/import_master_item_test.xlsx
+++ b/tests/Import/import_master_item_test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Point\point\tests\Import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\point\tests\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18EFD1C-3495-4E17-BE0C-5B51C212BC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7032"/>
+    <workbookView xWindow="4020" yWindow="3315" windowWidth="15375" windowHeight="8205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,19 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="38">
   <si>
     <t>No</t>
   </si>
@@ -142,12 +136,15 @@
   </si>
   <si>
     <t>%$%#</t>
+  </si>
+  <si>
+    <t>Pensil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -493,26 +490,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="7" max="8" width="17.88671875" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" customWidth="1"/>
-    <col min="10" max="10" width="31.21875" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="7" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" customWidth="1"/>
+    <col min="10" max="10" width="31.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -547,7 +544,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
@@ -555,7 +552,7 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -582,7 +579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
@@ -617,7 +614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>3</v>
       </c>
@@ -652,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>4</v>
       </c>
@@ -687,7 +684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>5</v>
       </c>
@@ -722,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>6</v>
       </c>
@@ -757,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>7</v>
       </c>
@@ -792,7 +789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>8</v>
       </c>
@@ -827,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>9</v>
       </c>
@@ -862,7 +859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>10</v>
       </c>
@@ -897,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>11</v>
       </c>
@@ -932,7 +929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>12</v>
       </c>
@@ -967,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>13</v>
       </c>
@@ -990,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>14</v>
       </c>

</xml_diff>